<commit_message>
la til force recomput i load_or_update
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ4"/>
+  <dimension ref="A1:AZ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,7 +698,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind----depth580-mstop10-run2.csv</t>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0200-freq1300-per15-depth580-mstop30-run1.csv</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -717,18 +717,24 @@
           <t>low</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>15</v>
+      </c>
       <c r="I2" t="n">
         <v>580</v>
       </c>
       <c r="J2" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -744,59 +750,117 @@
         <v>12545</v>
       </c>
       <c r="P2" t="n">
-        <v>273.46324</v>
+        <v>273.9290399999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>272.7732</v>
+        <v>272.7534400000001</v>
       </c>
       <c r="R2" t="n">
-        <v>273.2674</v>
+        <v>273.54304</v>
       </c>
       <c r="S2" t="n">
-        <v>273.94552</v>
-      </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
+        <v>273.9124</v>
+      </c>
+      <c r="T2" t="n">
+        <v>4500</v>
+      </c>
+      <c r="U2" t="n">
+        <v>4600</v>
+      </c>
+      <c r="V2" t="n">
+        <v>6300</v>
+      </c>
+      <c r="W2" t="n">
+        <v>6300</v>
+      </c>
+      <c r="X2" t="n">
+        <v>4884.615384615385</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>4984.615384615385</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>6684.615384615385</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>6684.615384615385</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>16.01499999999999</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>11.28858090714791</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>17.10899999999999</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>11.87856036196416</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>8.718600000000002</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>6.081144637714168</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>8.418600000000023</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>5.972338359796881</v>
+      </c>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr"/>
+      <c r="AL2" t="n">
+        <v>6.806142401044793</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.9231639505830895</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>17.83209309073736</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.1164462903394753</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>3.94756259260598</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.9992551669737394</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>1.200113135758016</v>
+      </c>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="inlineStr"/>
-      <c r="AW2" t="inlineStr"/>
-      <c r="AX2" t="inlineStr"/>
+      <c r="AU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>1.068310958476429</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.5095914431001231</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.965590805863329</v>
+      </c>
       <c r="AY2" t="inlineStr">
         <is>
           <t>20251110-tett6roof-lowMooring-2</t>
         </is>
       </c>
-      <c r="AZ2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0200-freq1300-per15-depth580-mstop30-run1.csv</t>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0100-freq1300-per15-depth580-mstop30-run1.csv</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -816,7 +880,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G3" t="n">
         <v>1.3</v>
@@ -848,16 +912,16 @@
         <v>12545</v>
       </c>
       <c r="P3" t="n">
-        <v>273.9290399999999</v>
+        <v>273.86156</v>
       </c>
       <c r="Q3" t="n">
-        <v>272.7534400000001</v>
+        <v>272.68212</v>
       </c>
       <c r="R3" t="n">
-        <v>273.54304</v>
+        <v>273.47164</v>
       </c>
       <c r="S3" t="n">
-        <v>273.9124</v>
+        <v>273.8552</v>
       </c>
       <c r="T3" t="n">
         <v>4500</v>
@@ -884,28 +948,28 @@
         <v>6684.615384615385</v>
       </c>
       <c r="AB3" t="n">
-        <v>16.01499999999999</v>
+        <v>8.624999999999972</v>
       </c>
       <c r="AC3" t="n">
-        <v>11.28858090714791</v>
+        <v>6.252911723343706</v>
       </c>
       <c r="AD3" t="n">
-        <v>17.10899999999999</v>
+        <v>9.055000000000007</v>
       </c>
       <c r="AE3" t="n">
-        <v>11.87856036196416</v>
+        <v>6.890160963712458</v>
       </c>
       <c r="AF3" t="n">
-        <v>8.718600000000002</v>
+        <v>4.423200000000012</v>
       </c>
       <c r="AG3" t="n">
-        <v>6.081144637714168</v>
+        <v>2.986366156897033</v>
       </c>
       <c r="AH3" t="n">
-        <v>8.418600000000023</v>
+        <v>4.338600000000007</v>
       </c>
       <c r="AI3" t="n">
-        <v>5.972338359796881</v>
+        <v>2.876624462536083</v>
       </c>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
@@ -919,7 +983,7 @@
         <v>17.83209309073736</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.1164462903394753</v>
+        <v>0.06162961944146066</v>
       </c>
       <c r="AP3" t="n">
         <v>3.94756259260598</v>
@@ -936,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="AV3" t="n">
-        <v>1.068310958476429</v>
+        <v>1.049855072463772</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.5095914431001231</v>
+        <v>0.4884815019326348</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.965590805863329</v>
+        <v>0.9808735756918057</v>
       </c>
       <c r="AY3" t="inlineStr">
         <is>
@@ -950,168 +1014,6 @@
         </is>
       </c>
       <c r="AZ3" t="inlineStr">
-        <is>
-          <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0100-freq1300-per15-depth580-mstop30-run1.csv</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>full</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>low</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="H4" t="n">
-        <v>15</v>
-      </c>
-      <c r="I4" t="n">
-        <v>580</v>
-      </c>
-      <c r="J4" t="n">
-        <v>30</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>8855</v>
-      </c>
-      <c r="M4" t="n">
-        <v>9455</v>
-      </c>
-      <c r="N4" t="n">
-        <v>12544</v>
-      </c>
-      <c r="O4" t="n">
-        <v>12545</v>
-      </c>
-      <c r="P4" t="n">
-        <v>273.86156</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>272.68212</v>
-      </c>
-      <c r="R4" t="n">
-        <v>273.47164</v>
-      </c>
-      <c r="S4" t="n">
-        <v>273.8552</v>
-      </c>
-      <c r="T4" t="n">
-        <v>4500</v>
-      </c>
-      <c r="U4" t="n">
-        <v>4600</v>
-      </c>
-      <c r="V4" t="n">
-        <v>6300</v>
-      </c>
-      <c r="W4" t="n">
-        <v>6300</v>
-      </c>
-      <c r="X4" t="n">
-        <v>4884.615384615385</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>4984.615384615385</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>6684.615384615385</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>6684.615384615385</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>8.624999999999972</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>6.252911723343706</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>9.055000000000007</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>6.890160963712458</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>4.423200000000012</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>2.986366156897033</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>4.338600000000007</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>2.876624462536083</v>
-      </c>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="n">
-        <v>6.806142401044793</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>0.9231639505830895</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>17.83209309073736</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0.06162961944146066</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>3.94756259260598</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>0.9992551669737394</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>1.200113135758016</v>
-      </c>
-      <c r="AS4" t="inlineStr"/>
-      <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV4" t="n">
-        <v>1.049855072463772</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>0.4884815019326348</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>0.9808735756918057</v>
-      </c>
-      <c r="AY4" t="inlineStr">
-        <is>
-          <t>20251110-tett6roof-lowMooring-2</t>
-        </is>
-      </c>
-      <c r="AZ4" t="inlineStr">
         <is>
           <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
         </is>

</xml_diff>

<commit_message>
data loader fikset. fjernet * fra input.
Signed-off-by: OleBB <oleb1996@gmail.com>
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:AZ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,7 +698,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0200-freq1300-per15-depth580-mstop30-run1.csv</t>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind----depth580-mstop10-run2.csv</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -717,24 +717,18 @@
           <t>low</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="H2" t="n">
-        <v>15</v>
-      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>580</v>
       </c>
       <c r="J2" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -750,117 +744,59 @@
         <v>12545</v>
       </c>
       <c r="P2" t="n">
-        <v>273.9290399999999</v>
+        <v>273.46324</v>
       </c>
       <c r="Q2" t="n">
-        <v>272.7534400000001</v>
+        <v>272.7732</v>
       </c>
       <c r="R2" t="n">
-        <v>273.54304</v>
+        <v>273.2674</v>
       </c>
       <c r="S2" t="n">
-        <v>273.9124</v>
-      </c>
-      <c r="T2" t="n">
-        <v>4500</v>
-      </c>
-      <c r="U2" t="n">
-        <v>4600</v>
-      </c>
-      <c r="V2" t="n">
-        <v>6300</v>
-      </c>
-      <c r="W2" t="n">
-        <v>6300</v>
-      </c>
-      <c r="X2" t="n">
-        <v>4884.615384615385</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>4984.615384615385</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>6684.615384615385</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>6684.615384615385</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>16.01499999999999</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>11.28858090714791</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>17.10899999999999</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>11.87856036196416</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>8.718600000000002</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>6.081144637714168</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>8.418600000000023</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>5.972338359796881</v>
-      </c>
+        <v>273.94552</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="n">
-        <v>6.806142401044793</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.9231639505830895</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>17.83209309073736</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.1164462903394753</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>3.94756259260598</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.9992551669737394</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>1.200113135758016</v>
-      </c>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>1.068310958476429</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0.5095914431001231</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>0.965590805863329</v>
-      </c>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
       <c r="AY2" t="inlineStr">
         <is>
           <t>20251110-tett6roof-lowMooring-2</t>
         </is>
       </c>
-      <c r="AZ2" t="inlineStr">
-        <is>
-          <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
-        </is>
-      </c>
+      <c r="AZ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0100-freq1300-per15-depth580-mstop30-run1.csv</t>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0200-freq1300-per15-depth580-mstop30-run1.csv</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -880,7 +816,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G3" t="n">
         <v>1.3</v>
@@ -912,16 +848,16 @@
         <v>12545</v>
       </c>
       <c r="P3" t="n">
-        <v>273.86156</v>
+        <v>273.9290399999999</v>
       </c>
       <c r="Q3" t="n">
-        <v>272.68212</v>
+        <v>272.7534400000001</v>
       </c>
       <c r="R3" t="n">
-        <v>273.47164</v>
+        <v>273.54304</v>
       </c>
       <c r="S3" t="n">
-        <v>273.8552</v>
+        <v>273.9124</v>
       </c>
       <c r="T3" t="n">
         <v>4500</v>
@@ -948,28 +884,28 @@
         <v>6684.615384615385</v>
       </c>
       <c r="AB3" t="n">
-        <v>8.624999999999972</v>
+        <v>16.01499999999999</v>
       </c>
       <c r="AC3" t="n">
-        <v>6.252911723343706</v>
+        <v>11.28858090714791</v>
       </c>
       <c r="AD3" t="n">
-        <v>9.055000000000007</v>
+        <v>17.10899999999999</v>
       </c>
       <c r="AE3" t="n">
-        <v>6.890160963712458</v>
+        <v>11.87856036196416</v>
       </c>
       <c r="AF3" t="n">
-        <v>4.423200000000012</v>
+        <v>8.718600000000002</v>
       </c>
       <c r="AG3" t="n">
-        <v>2.986366156897033</v>
+        <v>6.081144637714168</v>
       </c>
       <c r="AH3" t="n">
-        <v>4.338600000000007</v>
+        <v>8.418600000000023</v>
       </c>
       <c r="AI3" t="n">
-        <v>2.876624462536083</v>
+        <v>5.972338359796881</v>
       </c>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
@@ -983,7 +919,7 @@
         <v>17.83209309073736</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.06162961944146066</v>
+        <v>0.1164462903394753</v>
       </c>
       <c r="AP3" t="n">
         <v>3.94756259260598</v>
@@ -1000,20 +936,182 @@
         <v>0</v>
       </c>
       <c r="AV3" t="n">
+        <v>1.068310958476429</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0.5095914431001231</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.965590805863329</v>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>20251110-tett6roof-lowMooring-2</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>/Users/ole/Kodevik/wave_project/wavedata/20251110-tett6roof-lowMooring-2/fullpanel-nowind-amp0100-freq1300-per15-depth580-mstop30-run1.csv</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>15</v>
+      </c>
+      <c r="I4" t="n">
+        <v>580</v>
+      </c>
+      <c r="J4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>8855</v>
+      </c>
+      <c r="M4" t="n">
+        <v>9455</v>
+      </c>
+      <c r="N4" t="n">
+        <v>12544</v>
+      </c>
+      <c r="O4" t="n">
+        <v>12545</v>
+      </c>
+      <c r="P4" t="n">
+        <v>273.86156</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>272.68212</v>
+      </c>
+      <c r="R4" t="n">
+        <v>273.47164</v>
+      </c>
+      <c r="S4" t="n">
+        <v>273.8552</v>
+      </c>
+      <c r="T4" t="n">
+        <v>4500</v>
+      </c>
+      <c r="U4" t="n">
+        <v>4600</v>
+      </c>
+      <c r="V4" t="n">
+        <v>6300</v>
+      </c>
+      <c r="W4" t="n">
+        <v>6300</v>
+      </c>
+      <c r="X4" t="n">
+        <v>4884.615384615385</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>4984.615384615385</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>6684.615384615385</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>6684.615384615385</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>8.624999999999972</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>6.252911723343706</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>9.055000000000007</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>6.890160963712458</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>4.423200000000012</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>2.986366156897033</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>4.338600000000007</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>2.876624462536083</v>
+      </c>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="n">
+        <v>6.806142401044793</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.9231639505830895</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>17.83209309073736</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.06162961944146066</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>3.94756259260598</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.9992551669737394</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>1.200113135758016</v>
+      </c>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="n">
         <v>1.049855072463772</v>
       </c>
-      <c r="AW3" t="n">
+      <c r="AW4" t="n">
         <v>0.4884815019326348</v>
       </c>
-      <c r="AX3" t="n">
+      <c r="AX4" t="n">
         <v>0.9808735756918057</v>
       </c>
-      <c r="AY3" t="inlineStr">
+      <c r="AY4" t="inlineStr">
         <is>
           <t>20251110-tett6roof-lowMooring-2</t>
         </is>
       </c>
-      <c r="AZ3" t="inlineStr">
+      <c r="AZ4" t="inlineStr">
         <is>
           <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
         </is>

</xml_diff>

<commit_message>
kjørte claudes vektoriserte fysiske amplitudeberegning
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
@@ -844,25 +844,25 @@
       <c r="AN2" t="inlineStr"/>
       <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="n">
-        <v>6.806142401044793</v>
+        <v>6.80845382890728</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.9231639505830895</v>
+        <v>0.922850542145485</v>
       </c>
       <c r="AR2" t="n">
-        <v>17.83209309073736</v>
+        <v>17.83814903173707</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.1164462903394753</v>
+        <v>0.1164858365587746</v>
       </c>
       <c r="AT2" t="n">
-        <v>3.94756259260598</v>
+        <v>3.948903220766222</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.9992551669737394</v>
+        <v>0.9992571606462729</v>
       </c>
       <c r="AV2" t="n">
-        <v>1.200113135758016</v>
+        <v>1.19970570478913</v>
       </c>
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
@@ -1018,25 +1018,25 @@
       <c r="AN3" t="inlineStr"/>
       <c r="AO3" t="inlineStr"/>
       <c r="AP3" t="n">
-        <v>6.806142401044793</v>
+        <v>6.80845382890728</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.9231639505830895</v>
+        <v>0.922850542145485</v>
       </c>
       <c r="AR3" t="n">
-        <v>17.83209309073736</v>
+        <v>17.83814903173707</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.06162961944146066</v>
+        <v>0.06165054942075547</v>
       </c>
       <c r="AT3" t="n">
-        <v>3.94756259260598</v>
+        <v>3.948903220766222</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.9992551669737394</v>
+        <v>0.9992571606462729</v>
       </c>
       <c r="AV3" t="n">
-        <v>1.200113135758016</v>
+        <v>1.19970570478913</v>
       </c>
       <c r="AW3" t="inlineStr"/>
       <c r="AX3" t="inlineStr"/>

</xml_diff>

<commit_message>
oppgraderer fft og psd v grok
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD4"/>
+  <dimension ref="A1:BU4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,275 +441,360 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>experiment_folder</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>file_date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>WindCondition</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>TunnelCondition</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>PanelCondition</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Mooring</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>WaveAmplitudeInput [Volt]</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>WaveFrequencyInput [Hz]</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>WavePeriodInput</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>WaterDepth [mm]</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Extra seconds</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Run number</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Probe 1 mm from paddle</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Stillwater Probe 1</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Computed Probe 1 start</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Computed Probe 1 end</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 1 Amplitude</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 1 Amplitude (PSD)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 1 Amplitude (FFT)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 1 WavePeriod (FFT)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 1 Wavenumber (FFT)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 1 Wavelength (FFT)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 1 Significant Wave Height Hm0 (FFT)</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Probe 2 mm from paddle</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Stillwater Probe 2</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Computed Probe 2 start</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Computed Probe 2 end</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 2 Amplitude</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 2 Amplitude (PSD)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 2 Amplitude (FFT)</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 2 WavePeriod (FFT)</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 2 Wavenumber (FFT)</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 2 Wavelength (FFT)</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 2 Significant Wave Height Hm0 (FFT)</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Probe 3 mm from paddle</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Stillwater Probe 3</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Computed Probe 3 start</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Computed Probe 3 end</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 3 Amplitude</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 3 Amplitude (PSD)</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 3 Amplitude (FFT)</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 3 WavePeriod (FFT)</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 3 Wavenumber (FFT)</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 3 Wavelength (FFT)</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 3 Significant Wave Height Hm0 (FFT)</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Probe 4 mm from paddle</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Stillwater Probe 1</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Stillwater Probe 2</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Stillwater Probe 3</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Stillwater Probe 4</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Computed Probe 1 start</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Computed Probe 2 start</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Computed Probe 3 start</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Computed Probe 4 start</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Computed Probe 1 end</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Computed Probe 2 end</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Computed Probe 3 end</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Computed Probe 4 end</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 1 Amplitude</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 1 Amplitude (PSD)</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 1 Amplitude (FFT)</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 2 Amplitude</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 2 Amplitude (PSD)</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 2 Amplitude (FFT)</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 3 Amplitude</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 3 Amplitude (PSD)</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Probe 3 Amplitude (FFT)</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Probe 4 Amplitude</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Probe 4 Amplitude (PSD)</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Probe 4 Amplitude (FFT)</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 4 WavePeriod (FFT)</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 4 Wavenumber (FFT)</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 4 Wavelength (FFT)</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Probe 4 Significant Wave Height Hm0 (FFT)</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Wavefrequency</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Waveperiod</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Wavenumber</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Wavelength</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>kL</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>ak</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>kH</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>tanh(kH)</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>Celerity</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>Significant Wave Height Hs</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>Significant Wave Height Hm0</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>Windspeed</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>P2/P1</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>P3/P2</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>P4/P3</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
-        <is>
-          <t>experiment_folder</t>
-        </is>
-      </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>PROCESSED_folder</t>
         </is>
@@ -723,167 +808,188 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>20251110-tett6roof-lowMooring-2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-11-10T15:25:36</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>full</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>low</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>0.2</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>1.3</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>15</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>580</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>30</v>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="L2" t="n">
-        <v>8855</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O2" t="n">
+        <v>273.9290399999999</v>
+      </c>
+      <c r="P2" t="n">
+        <v>4500</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>4884.615384615385</v>
+      </c>
+      <c r="R2" t="n">
+        <v>16.01499999999999</v>
+      </c>
+      <c r="S2" t="n">
+        <v>11.28858090714791</v>
+      </c>
+      <c r="T2" t="n">
+        <v>14.4627525192995</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="n">
         <v>9455</v>
       </c>
-      <c r="N2" t="n">
+      <c r="Z2" t="n">
+        <v>272.7534400000001</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>4600</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>4984.615384615385</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>17.10899999999999</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>11.87856036196416</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>14.70048585559625</v>
+      </c>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="n">
         <v>12544</v>
       </c>
-      <c r="O2" t="n">
+      <c r="AK2" t="n">
+        <v>273.54304</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>6300</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>6684.615384615385</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>8.718600000000002</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>6.081144637714168</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>7.851476346848065</v>
+      </c>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="n">
         <v>12545</v>
       </c>
-      <c r="P2" t="n">
-        <v>273.9290399999999</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>272.7534400000001</v>
-      </c>
-      <c r="R2" t="n">
-        <v>273.54304</v>
-      </c>
-      <c r="S2" t="n">
+      <c r="AV2" t="n">
         <v>273.9124</v>
       </c>
-      <c r="T2" t="n">
-        <v>4500</v>
-      </c>
-      <c r="U2" t="n">
-        <v>4600</v>
-      </c>
-      <c r="V2" t="n">
+      <c r="AW2" t="n">
         <v>6300</v>
       </c>
-      <c r="W2" t="n">
-        <v>6300</v>
-      </c>
-      <c r="X2" t="n">
-        <v>4884.615384615385</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>4984.615384615385</v>
-      </c>
-      <c r="Z2" t="n">
+      <c r="AX2" t="n">
         <v>6684.615384615385</v>
       </c>
-      <c r="AA2" t="n">
-        <v>6684.615384615385</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>16.01499999999999</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>11.28858090714791</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>14.4627525192995</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>17.10899999999999</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>11.87856036196416</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>14.70048585559625</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>8.718600000000002</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>6.081144637714168</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>7.851476346848065</v>
-      </c>
-      <c r="AK2" t="n">
+      <c r="AY2" t="n">
         <v>8.418600000000023</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AZ2" t="n">
         <v>5.972338359796881</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="BA2" t="n">
         <v>7.654156016951084</v>
       </c>
-      <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="n">
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="n">
         <v>6.80845382890728</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="BI2" t="n">
         <v>0.922850542145485</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="BJ2" t="n">
         <v>17.83814903173707</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="BK2" t="n">
         <v>0.1164858365587746</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="BL2" t="n">
         <v>3.948903220766222</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="BM2" t="n">
         <v>0.9992571606462729</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="BN2" t="n">
         <v>1.19970570478913</v>
       </c>
-      <c r="AW2" t="inlineStr"/>
-      <c r="AX2" t="inlineStr"/>
-      <c r="AY2" t="n">
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="n">
         <v>0</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="BR2" t="n">
         <v>1.068310958476429</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BS2" t="n">
         <v>0.5095914431001231</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BT2" t="n">
         <v>0.965590805863329</v>
       </c>
-      <c r="BC2" t="inlineStr">
-        <is>
-          <t>20251110-tett6roof-lowMooring-2</t>
-        </is>
-      </c>
-      <c r="BD2" t="inlineStr">
+      <c r="BU2" t="inlineStr">
         <is>
           <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
         </is>
@@ -897,167 +1003,188 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>20251110-tett6roof-lowMooring-2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-11-10T15:07:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>full</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>low</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>0.1</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>1.3</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>15</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>580</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>30</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="L3" t="n">
-        <v>8855</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O3" t="n">
+        <v>273.86156</v>
+      </c>
+      <c r="P3" t="n">
+        <v>4500</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>4884.615384615385</v>
+      </c>
+      <c r="R3" t="n">
+        <v>8.624999999999972</v>
+      </c>
+      <c r="S3" t="n">
+        <v>6.252911723343706</v>
+      </c>
+      <c r="T3" t="n">
+        <v>7.885542681084842</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="n">
         <v>9455</v>
       </c>
-      <c r="N3" t="n">
+      <c r="Z3" t="n">
+        <v>272.68212</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>4600</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>4984.615384615385</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>9.055000000000007</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>6.890160963712458</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>8.253703056623822</v>
+      </c>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="n">
         <v>12544</v>
       </c>
-      <c r="O3" t="n">
+      <c r="AK3" t="n">
+        <v>273.47164</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>6300</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>6684.615384615385</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>4.423200000000012</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>2.986366156897033</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>3.700572463528926</v>
+      </c>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="n">
         <v>12545</v>
       </c>
-      <c r="P3" t="n">
-        <v>273.86156</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>272.68212</v>
-      </c>
-      <c r="R3" t="n">
-        <v>273.47164</v>
-      </c>
-      <c r="S3" t="n">
+      <c r="AV3" t="n">
         <v>273.8552</v>
       </c>
-      <c r="T3" t="n">
-        <v>4500</v>
-      </c>
-      <c r="U3" t="n">
-        <v>4600</v>
-      </c>
-      <c r="V3" t="n">
+      <c r="AW3" t="n">
         <v>6300</v>
       </c>
-      <c r="W3" t="n">
-        <v>6300</v>
-      </c>
-      <c r="X3" t="n">
-        <v>4884.615384615385</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>4984.615384615385</v>
-      </c>
-      <c r="Z3" t="n">
+      <c r="AX3" t="n">
         <v>6684.615384615385</v>
       </c>
-      <c r="AA3" t="n">
-        <v>6684.615384615385</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>8.624999999999972</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>6.252911723343706</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>7.885542681084842</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>9.055000000000007</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>6.890160963712458</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>8.253703056623822</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>4.423200000000012</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>2.986366156897033</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>3.700572463528926</v>
-      </c>
-      <c r="AK3" t="n">
+      <c r="AY3" t="n">
         <v>4.338600000000007</v>
       </c>
-      <c r="AL3" t="n">
+      <c r="AZ3" t="n">
         <v>2.876624462536083</v>
       </c>
-      <c r="AM3" t="n">
+      <c r="BA3" t="n">
         <v>3.506697885574963</v>
       </c>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="n">
+      <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="inlineStr"/>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr"/>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr"/>
+      <c r="BH3" t="n">
         <v>6.80845382890728</v>
       </c>
-      <c r="AQ3" t="n">
+      <c r="BI3" t="n">
         <v>0.922850542145485</v>
       </c>
-      <c r="AR3" t="n">
+      <c r="BJ3" t="n">
         <v>17.83814903173707</v>
       </c>
-      <c r="AS3" t="n">
+      <c r="BK3" t="n">
         <v>0.06165054942075547</v>
       </c>
-      <c r="AT3" t="n">
+      <c r="BL3" t="n">
         <v>3.948903220766222</v>
       </c>
-      <c r="AU3" t="n">
+      <c r="BM3" t="n">
         <v>0.9992571606462729</v>
       </c>
-      <c r="AV3" t="n">
+      <c r="BN3" t="n">
         <v>1.19970570478913</v>
       </c>
-      <c r="AW3" t="inlineStr"/>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="n">
+      <c r="BO3" t="inlineStr"/>
+      <c r="BP3" t="inlineStr"/>
+      <c r="BQ3" t="n">
         <v>0</v>
       </c>
-      <c r="AZ3" t="n">
+      <c r="BR3" t="n">
         <v>1.049855072463772</v>
       </c>
-      <c r="BA3" t="n">
+      <c r="BS3" t="n">
         <v>0.4884815019326348</v>
       </c>
-      <c r="BB3" t="n">
+      <c r="BT3" t="n">
         <v>0.9808735756918057</v>
       </c>
-      <c r="BC3" t="inlineStr">
-        <is>
-          <t>20251110-tett6roof-lowMooring-2</t>
-        </is>
-      </c>
-      <c r="BD3" t="inlineStr">
+      <c r="BU3" t="inlineStr">
         <is>
           <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
         </is>
@@ -1071,133 +1198,154 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>20251110-tett6roof-lowMooring-2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-11-10T15:00:24</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>full</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>low</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
         <v>580</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>10</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="L4" t="n">
-        <v>8855</v>
-      </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
+        <v>18000</v>
+      </c>
+      <c r="O4" t="n">
+        <v>273.46324</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>6249</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.6599999999999966</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="n">
         <v>9455</v>
       </c>
-      <c r="N4" t="n">
-        <v>12544</v>
-      </c>
-      <c r="O4" t="n">
-        <v>12545</v>
-      </c>
-      <c r="P4" t="n">
-        <v>273.46324</v>
-      </c>
-      <c r="Q4" t="n">
+      <c r="Z4" t="n">
         <v>272.7732</v>
       </c>
-      <c r="R4" t="n">
-        <v>273.2674</v>
-      </c>
-      <c r="S4" t="n">
-        <v>273.94552</v>
-      </c>
-      <c r="T4" t="n">
+      <c r="AA4" t="n">
         <v>0</v>
       </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" t="n">
+      <c r="AB4" t="n">
         <v>6249</v>
       </c>
-      <c r="Y4" t="n">
-        <v>6249</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>6249</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>6249</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.6599999999999966</v>
-      </c>
-      <c r="AC4" t="inlineStr"/>
+      <c r="AC4" t="n">
+        <v>0.9099999999999966</v>
+      </c>
       <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="n">
-        <v>0.9099999999999966</v>
-      </c>
+      <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="n">
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="n">
+        <v>12544</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>273.2674</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>6249</v>
+      </c>
+      <c r="AN4" t="n">
         <v>0.5550000000000068</v>
       </c>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="n">
-        <v>0.6999999999999886</v>
-      </c>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr"/>
       <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="n">
-        <v>0</v>
-      </c>
+      <c r="AP4" t="inlineStr"/>
       <c r="AQ4" t="inlineStr"/>
       <c r="AR4" t="inlineStr"/>
       <c r="AS4" t="inlineStr"/>
       <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr"/>
-      <c r="AV4" t="inlineStr"/>
-      <c r="AW4" t="inlineStr"/>
-      <c r="AX4" t="inlineStr"/>
+      <c r="AU4" t="n">
+        <v>12545</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>273.94552</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>6249</v>
+      </c>
       <c r="AY4" t="n">
+        <v>0.6999999999999886</v>
+      </c>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="n">
         <v>0</v>
       </c>
-      <c r="AZ4" t="n">
+      <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR4" t="n">
         <v>1.378787878787881</v>
       </c>
-      <c r="BA4" t="n">
+      <c r="BS4" t="n">
         <v>0.6098901098901197</v>
       </c>
-      <c r="BB4" t="n">
+      <c r="BT4" t="n">
         <v>1.261261261261225</v>
       </c>
-      <c r="BC4" t="inlineStr">
-        <is>
-          <t>20251110-tett6roof-lowMooring-2</t>
-        </is>
-      </c>
-      <c r="BD4" t="inlineStr">
+      <c r="BU4" t="inlineStr">
         <is>
           <t>PROCESSED-20251110-tett6roof-lowMooring-2</t>
         </is>

</xml_diff>

<commit_message>
nu, skille sweell og wind, og plotte som i damping-grouped
</commit_message>
<xml_diff>
--- a/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
+++ b/waveprocessed/PROCESSED-20251110-tett6roof-lowMooring-2/meta.xlsx
@@ -859,19 +859,19 @@
         <v>273.9290399999999</v>
       </c>
       <c r="P2" t="n">
-        <v>4500</v>
+        <v>4600</v>
       </c>
       <c r="Q2" t="n">
-        <v>4884.615384615385</v>
+        <v>4984.615384615385</v>
       </c>
       <c r="R2" t="n">
-        <v>16.01499999999999</v>
+        <v>17.30039999999998</v>
       </c>
       <c r="S2" t="n">
-        <v>11.28858090714791</v>
+        <v>12.40840678741196</v>
       </c>
       <c r="T2" t="n">
-        <v>14.4627525192995</v>
+        <v>15.28740162368884</v>
       </c>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
@@ -884,19 +884,19 @@
         <v>272.7534400000001</v>
       </c>
       <c r="AA2" t="n">
-        <v>4600</v>
+        <v>4700</v>
       </c>
       <c r="AB2" t="n">
-        <v>4984.615384615385</v>
+        <v>5084.615384615385</v>
       </c>
       <c r="AC2" t="n">
-        <v>17.10899999999999</v>
+        <v>15.26759999999998</v>
       </c>
       <c r="AD2" t="n">
-        <v>11.87856036196416</v>
+        <v>11.20950937555914</v>
       </c>
       <c r="AE2" t="n">
-        <v>14.70048585559625</v>
+        <v>14.1811631901298</v>
       </c>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="inlineStr"/>
@@ -909,19 +909,19 @@
         <v>273.54304</v>
       </c>
       <c r="AL2" t="n">
-        <v>6300</v>
+        <v>6400</v>
       </c>
       <c r="AM2" t="n">
-        <v>6684.615384615385</v>
+        <v>6784.615384615385</v>
       </c>
       <c r="AN2" t="n">
-        <v>8.718600000000002</v>
+        <v>9.407200000000003</v>
       </c>
       <c r="AO2" t="n">
-        <v>6.081144637714168</v>
+        <v>6.698401312054257</v>
       </c>
       <c r="AP2" t="n">
-        <v>7.851476346848065</v>
+        <v>8.30968077669284</v>
       </c>
       <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="inlineStr"/>
@@ -934,19 +934,19 @@
         <v>273.9124</v>
       </c>
       <c r="AW2" t="n">
-        <v>6300</v>
+        <v>6400</v>
       </c>
       <c r="AX2" t="n">
-        <v>6684.615384615385</v>
+        <v>6784.615384615385</v>
       </c>
       <c r="AY2" t="n">
-        <v>8.418600000000023</v>
+        <v>9.325400000000027</v>
       </c>
       <c r="AZ2" t="n">
-        <v>5.972338359796881</v>
+        <v>6.51790130812388</v>
       </c>
       <c r="BA2" t="n">
-        <v>7.654156016951084</v>
+        <v>8.131027086979174</v>
       </c>
       <c r="BB2" t="inlineStr"/>
       <c r="BC2" t="inlineStr"/>
@@ -964,7 +964,7 @@
         <v>17.83814903173707</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.1164858365587746</v>
+        <v>0.1039487496782247</v>
       </c>
       <c r="BL2" t="n">
         <v>3.948903220766222</v>
@@ -981,13 +981,13 @@
         <v>0</v>
       </c>
       <c r="BR2" t="n">
-        <v>1.068310958476429</v>
+        <v>0.8824998265936047</v>
       </c>
       <c r="BS2" t="n">
-        <v>0.5095914431001231</v>
+        <v>0.6161544709057097</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.965590805863329</v>
+        <v>0.9913045326983613</v>
       </c>
       <c r="BU2" t="inlineStr">
         <is>
@@ -1054,19 +1054,19 @@
         <v>273.86156</v>
       </c>
       <c r="P3" t="n">
-        <v>4500</v>
+        <v>4600</v>
       </c>
       <c r="Q3" t="n">
-        <v>4884.615384615385</v>
+        <v>4984.615384615385</v>
       </c>
       <c r="R3" t="n">
-        <v>8.624999999999972</v>
+        <v>8.194999999999965</v>
       </c>
       <c r="S3" t="n">
-        <v>6.252911723343706</v>
+        <v>6.150988042443566</v>
       </c>
       <c r="T3" t="n">
-        <v>7.885542681084842</v>
+        <v>7.680335855956333</v>
       </c>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
@@ -1079,19 +1079,19 @@
         <v>272.68212</v>
       </c>
       <c r="AA3" t="n">
-        <v>4600</v>
+        <v>4700</v>
       </c>
       <c r="AB3" t="n">
-        <v>4984.615384615385</v>
+        <v>5084.615384615385</v>
       </c>
       <c r="AC3" t="n">
-        <v>9.055000000000007</v>
+        <v>8.625000000000028</v>
       </c>
       <c r="AD3" t="n">
-        <v>6.890160963712458</v>
+        <v>6.572803824607096</v>
       </c>
       <c r="AE3" t="n">
-        <v>8.253703056623822</v>
+        <v>7.985192377663065</v>
       </c>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="inlineStr"/>
@@ -1104,19 +1104,19 @@
         <v>273.47164</v>
       </c>
       <c r="AL3" t="n">
-        <v>6300</v>
+        <v>6400</v>
       </c>
       <c r="AM3" t="n">
-        <v>6684.615384615385</v>
+        <v>6784.615384615385</v>
       </c>
       <c r="AN3" t="n">
-        <v>4.423200000000012</v>
+        <v>4.041800000000021</v>
       </c>
       <c r="AO3" t="n">
-        <v>2.986366156897033</v>
+        <v>2.735792981627788</v>
       </c>
       <c r="AP3" t="n">
-        <v>3.700572463528926</v>
+        <v>3.530943225084268</v>
       </c>
       <c r="AQ3" t="inlineStr"/>
       <c r="AR3" t="inlineStr"/>
@@ -1129,19 +1129,19 @@
         <v>273.8552</v>
       </c>
       <c r="AW3" t="n">
-        <v>6300</v>
+        <v>6400</v>
       </c>
       <c r="AX3" t="n">
-        <v>6684.615384615385</v>
+        <v>6784.615384615385</v>
       </c>
       <c r="AY3" t="n">
-        <v>4.338600000000007</v>
+        <v>4.175400000000018</v>
       </c>
       <c r="AZ3" t="n">
-        <v>2.876624462536083</v>
+        <v>2.644811568780587</v>
       </c>
       <c r="BA3" t="n">
-        <v>3.506697885574963</v>
+        <v>3.371432832357906</v>
       </c>
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
         <v>17.83814903173707</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.06165054942075547</v>
+        <v>0.05872291427432548</v>
       </c>
       <c r="BL3" t="n">
         <v>3.948903220766222</v>
@@ -1176,13 +1176,13 @@
         <v>0</v>
       </c>
       <c r="BR3" t="n">
-        <v>1.049855072463772</v>
+        <v>1.05247101891398</v>
       </c>
       <c r="BS3" t="n">
-        <v>0.4884815019326348</v>
+        <v>0.468614492753624</v>
       </c>
       <c r="BT3" t="n">
-        <v>0.9808735756918057</v>
+        <v>1.033054579642732</v>
       </c>
       <c r="BU3" t="inlineStr">
         <is>

</xml_diff>